<commit_message>
fix missing edition in Mireya
</commit_message>
<xml_diff>
--- a/parser/public/data/MetaEdiciones.xlsx
+++ b/parser/public/data/MetaEdiciones.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26215"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10319"/>
   <workbookPr showInkAnnotation="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/juan/dev/lab/mujeres-de-prensa/parser/public/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/soporte/lab/mujeres-de-prensa/parser/public/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{014C6A66-A2F2-0640-BBF4-72C3D49D34BC}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="49600" yWindow="2540" windowWidth="27360" windowHeight="15820" tabRatio="500" activeTab="3"/>
+    <workbookView xWindow="11040" yWindow="2540" windowWidth="27360" windowHeight="15820" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Mireya" sheetId="1" r:id="rId1"/>
@@ -19,7 +20,7 @@
     <sheet name="Contrastes" sheetId="5" r:id="rId5"/>
     <sheet name="Mujer" sheetId="6" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="150000" concurrentCalc="0"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -29,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="164">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="165">
   <si>
     <t>Volumen</t>
   </si>
@@ -521,12 +522,15 @@
   </si>
   <si>
     <t>No.24</t>
+  </si>
+  <si>
+    <t>No.9/Jun/1944</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -576,6 +580,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -843,11 +850,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D23"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:D24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -873,7 +880,7 @@
         <v>Oct</v>
       </c>
       <c r="C2" t="str">
-        <f t="shared" ref="C2:C23" si="0">RIGHT(D2, 4)</f>
+        <f t="shared" ref="C2:C24" si="0">RIGHT(D2, 4)</f>
         <v>1943</v>
       </c>
       <c r="D2" t="s">
@@ -882,11 +889,11 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="str">
-        <f t="shared" ref="A3:A23" si="1">SUBSTITUTE(LEFT(D3,FIND("/",D3) - 1), "No.", "",1)</f>
+        <f t="shared" ref="A3:A24" si="1">SUBSTITUTE(LEFT(D3,FIND("/",D3) - 1), "No.", "",1)</f>
         <v>3</v>
       </c>
       <c r="B3" t="str">
-        <f t="shared" ref="B3:B23" si="2">MID(D3, FIND("/", D3) + 1, FIND( "!", SUBSTITUTE(D3, "/", "!", 2) ) - 2 - FIND("/", D3) + 1 )</f>
+        <f t="shared" ref="B3:B24" si="2">MID(D3, FIND("/", D3) + 1, FIND( "!", SUBSTITUTE(D3, "/", "!", 2) ) - 2 - FIND("/", D3) + 1 )</f>
         <v>Dic</v>
       </c>
       <c r="C3" t="str">
@@ -968,272 +975,289 @@
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" t="str">
         <f t="shared" si="1"/>
-        <v>10 y 11</v>
+        <v>9</v>
       </c>
       <c r="B8" t="str">
         <f t="shared" si="2"/>
-        <v>Jul y Ago</v>
+        <v>Jun</v>
       </c>
       <c r="C8" t="str">
         <f t="shared" si="0"/>
         <v>1944</v>
       </c>
       <c r="D8" t="s">
-        <v>9</v>
+        <v>164</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" t="str">
         <f t="shared" si="1"/>
-        <v>12</v>
+        <v>10 y 11</v>
       </c>
       <c r="B9" t="str">
         <f t="shared" si="2"/>
-        <v>Sep</v>
+        <v>Jul y Ago</v>
       </c>
       <c r="C9" t="str">
         <f t="shared" si="0"/>
         <v>1944</v>
       </c>
       <c r="D9" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" t="str">
         <f t="shared" si="1"/>
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B10" t="str">
         <f t="shared" si="2"/>
-        <v>Nov</v>
+        <v>Sep</v>
       </c>
       <c r="C10" t="str">
         <f t="shared" si="0"/>
         <v>1944</v>
       </c>
       <c r="D10" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" t="str">
         <f t="shared" si="1"/>
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B11" t="str">
         <f t="shared" si="2"/>
-        <v>Dic</v>
+        <v>Nov</v>
       </c>
       <c r="C11" t="str">
         <f t="shared" si="0"/>
         <v>1944</v>
       </c>
       <c r="D11" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" t="str">
         <f t="shared" si="1"/>
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B12" t="str">
         <f t="shared" si="2"/>
-        <v>Ene</v>
+        <v>Dic</v>
       </c>
       <c r="C12" t="str">
         <f t="shared" si="0"/>
-        <v>1945</v>
+        <v>1944</v>
       </c>
       <c r="D12" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" t="str">
         <f t="shared" si="1"/>
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B13" t="str">
         <f t="shared" si="2"/>
-        <v>Feb</v>
+        <v>Ene</v>
       </c>
       <c r="C13" t="str">
         <f t="shared" si="0"/>
         <v>1945</v>
       </c>
       <c r="D13" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" t="str">
         <f t="shared" si="1"/>
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B14" t="str">
         <f t="shared" si="2"/>
-        <v>Abr</v>
+        <v>Feb</v>
       </c>
       <c r="C14" t="str">
         <f t="shared" si="0"/>
         <v>1945</v>
       </c>
       <c r="D14" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" t="str">
         <f t="shared" si="1"/>
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B15" t="str">
         <f t="shared" si="2"/>
-        <v>May</v>
+        <v>Abr</v>
       </c>
       <c r="C15" t="str">
         <f t="shared" si="0"/>
         <v>1945</v>
       </c>
       <c r="D15" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" t="str">
         <f t="shared" si="1"/>
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B16" t="str">
         <f t="shared" si="2"/>
-        <v>Jun</v>
+        <v>May</v>
       </c>
       <c r="C16" t="str">
         <f t="shared" si="0"/>
         <v>1945</v>
       </c>
       <c r="D16" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" t="str">
         <f t="shared" si="1"/>
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B17" t="str">
         <f t="shared" si="2"/>
-        <v>Jul</v>
+        <v>Jun</v>
       </c>
       <c r="C17" t="str">
         <f t="shared" si="0"/>
         <v>1945</v>
       </c>
       <c r="D17" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" t="str">
         <f t="shared" si="1"/>
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B18" t="str">
         <f t="shared" si="2"/>
-        <v>Ago</v>
+        <v>Jul</v>
       </c>
       <c r="C18" t="str">
         <f t="shared" si="0"/>
         <v>1945</v>
       </c>
       <c r="D18" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" t="str">
         <f t="shared" si="1"/>
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B19" t="str">
         <f t="shared" si="2"/>
-        <v>Oct</v>
+        <v>Ago</v>
       </c>
       <c r="C19" t="str">
         <f t="shared" si="0"/>
         <v>1945</v>
       </c>
       <c r="D19" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" t="str">
         <f t="shared" si="1"/>
-        <v>23 y 24</v>
+        <v>22</v>
       </c>
       <c r="B20" t="str">
         <f t="shared" si="2"/>
-        <v>Nov y Dic</v>
+        <v>Oct</v>
       </c>
       <c r="C20" t="str">
         <f t="shared" si="0"/>
         <v>1945</v>
       </c>
       <c r="D20" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" t="str">
         <f t="shared" si="1"/>
-        <v>25</v>
+        <v>23 y 24</v>
       </c>
       <c r="B21" t="str">
         <f t="shared" si="2"/>
-        <v>Abr</v>
+        <v>Nov y Dic</v>
       </c>
       <c r="C21" t="str">
         <f t="shared" si="0"/>
-        <v>1946</v>
+        <v>1945</v>
       </c>
       <c r="D21" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" t="str">
         <f t="shared" si="1"/>
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B22" t="str">
         <f t="shared" si="2"/>
-        <v>Sep</v>
+        <v>Abr</v>
       </c>
       <c r="C22" t="str">
         <f t="shared" si="0"/>
         <v>1946</v>
       </c>
       <c r="D22" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" t="str">
         <f t="shared" si="1"/>
+        <v>26</v>
+      </c>
+      <c r="B23" t="str">
+        <f t="shared" si="2"/>
+        <v>Sep</v>
+      </c>
+      <c r="C23" t="str">
+        <f t="shared" si="0"/>
+        <v>1946</v>
+      </c>
+      <c r="D23" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A24" t="str">
+        <f t="shared" si="1"/>
         <v>27</v>
       </c>
-      <c r="B23" t="str">
+      <c r="B24" t="str">
         <f t="shared" si="2"/>
         <v>Oct</v>
       </c>
-      <c r="C23" t="str">
+      <c r="C24" t="str">
         <f t="shared" si="0"/>
         <v>1946</v>
       </c>
-      <c r="D23" t="s">
+      <c r="D24" t="s">
         <v>24</v>
       </c>
     </row>
@@ -1243,7 +1267,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1592,7 +1616,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:D24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2009,10 +2033,10 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:D25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
@@ -2227,7 +2251,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2338,7 +2362,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:D69"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>